<commit_message>
updated files after additional employer standardization step
</commit_message>
<xml_diff>
--- a/output/agencyreviewteams.xlsx
+++ b/output/agencyreviewteams.xlsx
@@ -820,7 +820,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>JUSTICE CATALYST LAW INC</t>
+          <t>JUSTICE CATALYST LAW</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>LATHAM &amp; WATKINS LLP</t>
+          <t>LATHAM &amp; WATKINS</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CLARK GROUP LLC</t>
+          <t>CLARK GROUP</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>CLIFFORD CHANCE US LLP</t>
+          <t>CLIFFORD CHANCE US</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>WILEY REIN LLP</t>
+          <t>WILEY REIN</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>CNKINDER INC</t>
+          <t>CNKINDER</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>GLOBAL COUNSEL LLC</t>
+          <t>GLOBAL COUNSEL</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>VISA INC</t>
+          <t>VISA</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>MANATT PHELPS AND PHILLIPS LLP</t>
+          <t>MANATT PHELPS AND PHILLIPS</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>OTHERSIDE CONSULTING LLC</t>
+          <t>OTHERSIDE CONSULTING</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>IMBUE GROUP INC</t>
+          <t>IMBUE GROUP</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>CACI INTERNATIONAL INC</t>
+          <t>CACI INTERNATIONAL</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>CLOUDFLARE INC</t>
+          <t>CLOUDFLARE</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>SENSHI AME ADVISORS LLC</t>
+          <t>SENSHI AME ADVISORS</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>INSTITUTE OF ELECTRONIC AND ELECTRICAL ENGINEERS INC</t>
+          <t>INSTITUTE OF ELECTRONIC AND ELECTRICAL ENGINEERS</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3284,7 +3284,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>TEACH PLUS INC</t>
+          <t>TEACH PLUS</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>RABEN GROUP LLC</t>
+          <t>RABEN GROUP</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>HIGH WATER MARK LLC</t>
+          <t>HIGH WATER MARK</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -3964,7 +3964,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>BFPCC INC</t>
+          <t>BFPCC</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -3996,7 +3996,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>MANATT PHELPS AND PHILLIPS LLP</t>
+          <t>MANATT PHELPS AND PHILLIPS</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>BOIES SCHILLER FLEXNER LLP</t>
+          <t>BOIES SCHILLER FLEXNER</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>HOGAN LOVELLS LLP</t>
+          <t>HOGAN LOVELLS</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>INSTITUTES FOR BEHAVIOR RESOURCES INC</t>
+          <t>INSTITUTES FOR BEHAVIOR RESOURCES</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>GUIDEHOUSE INC</t>
+          <t>GUIDEHOUSE</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>MANATT PHELPS AND PHILLIPS LLP</t>
+          <t>MANATT PHELPS AND PHILLIPS</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>TOFFLER ASSOCIATES INC</t>
+          <t>TOFFLER ASSOCIATES</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>ONE CONCERN INC</t>
+          <t>ONE CONCERN</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>SHEPPARD MULLIN RICHTER &amp; HAMPTON LLP</t>
+          <t>SHEPPARD MULLIN RICHTER &amp; HAMPTON</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>LEVY GROUP INC</t>
+          <t>LEVY GROUP</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>CROWELL &amp; MORING LLP</t>
+          <t>CROWELL &amp; MORING</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>PAUL HASTINGS LLP</t>
+          <t>PAUL HASTINGS</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -6067,7 +6067,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>ADVOCACY BLUEPRINTS LLC</t>
+          <t>ADVOCACY BLUEPRINTS</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>HARRIS WILTSHIRE AND GRANNIS LLP</t>
+          <t>HARRIS WILTSHIRE AND GRANNIS</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -6789,7 +6789,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>LINKLATERS LLP</t>
+          <t>LINKLATERS</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -6816,7 +6816,7 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>LATHAM &amp; WATKINS LLP</t>
+          <t>LATHAM &amp; WATKINS</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -6870,7 +6870,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>ARNOLD VENTURES LLC</t>
+          <t>ARNOLD VENTURES</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -6924,7 +6924,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>WILMERHALE LLC</t>
+          <t>WILMERHALE</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>MAYER BROWN LLP</t>
+          <t>MAYER BROWN</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -6978,7 +6978,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>MORGAN LEWIS &amp; BOCKIUS LLP</t>
+          <t>MORGAN LEWIS &amp; BOCKIUS</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>COOLEY LLP</t>
+          <t>COOLEY</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -7248,7 +7248,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>DAVIS POLK &amp; WARDWELL LLP</t>
+          <t>DAVIS POLK &amp; WARDWELL</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -7491,7 +7491,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>HUNTON ANDREWS KURTH LLP</t>
+          <t>HUNTON ANDREWS KURTH</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -8198,7 +8198,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>JOBS FOR THE FUTURE INC</t>
+          <t>JOBS FOR THE FUTURE</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -8834,7 +8834,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>HWC INC</t>
+          <t>HWC</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>FACEBOOK INC</t>
+          <t>FACEBOOK</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -9620,7 +9620,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>SKADDEN ARPS SLATE MEAGHER &amp; FLOM LLP</t>
+          <t>SKADDEN ARPS SLATE MEAGHER &amp; FLOM</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -9733,7 +9733,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>INTERNATIONAL CAPITAL STRATEGIES LLC</t>
+          <t>INTERNATIONAL CAPITAL STRATEGIES</t>
         </is>
       </c>
       <c r="H335" t="inlineStr">
@@ -10013,7 +10013,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>BRIGHTSIDE BENEFIT INC</t>
+          <t>BRIGHTSIDE BENEFIT</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -10266,7 +10266,7 @@
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>ARNOLD &amp; PORTER KAYE SCHOLER LLP</t>
+          <t>ARNOLD &amp; PORTER KAYE SCHOLER</t>
         </is>
       </c>
       <c r="H354" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>ATLAS RESEARCH LLC</t>
+          <t>ATLAS RESEARCH</t>
         </is>
       </c>
       <c r="H377" t="inlineStr">
@@ -11204,7 +11204,7 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>WORKMERK LLC</t>
+          <t>WORKMERK</t>
         </is>
       </c>
       <c r="H388" t="inlineStr">
@@ -11398,7 +11398,7 @@
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>LATHAM &amp; WATKINS LLP</t>
+          <t>LATHAM &amp; WATKINS</t>
         </is>
       </c>
       <c r="H395" t="inlineStr">
@@ -11425,7 +11425,7 @@
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>GRIST MAGAZINE INC</t>
+          <t>GRIST MAGAZINE</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -11877,7 +11877,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>DLA PIPER LLP</t>
+          <t>DLA PIPER</t>
         </is>
       </c>
       <c r="H412" t="inlineStr">
@@ -12194,7 +12194,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>BETTER MARKETS INC</t>
+          <t>BETTER MARKETS</t>
         </is>
       </c>
       <c r="H423" t="inlineStr">
@@ -12334,7 +12334,7 @@
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>ORRICK HERRINGTON &amp; SUTCLIFFE LLP</t>
+          <t>ORRICK HERRINGTON &amp; SUTCLIFFE</t>
         </is>
       </c>
       <c r="H428" t="inlineStr">
@@ -12457,7 +12457,7 @@
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>ELEVATE LLC</t>
+          <t>ELEVATE</t>
         </is>
       </c>
       <c r="H432" t="inlineStr">
@@ -12592,7 +12592,7 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>CLIO STRATEGIES LLC</t>
+          <t>CLIO STRATEGIES</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
@@ -12958,7 +12958,7 @@
       </c>
       <c r="F450" t="inlineStr">
         <is>
-          <t>FACEBOOK INC</t>
+          <t>FACEBOOK</t>
         </is>
       </c>
       <c r="H450" t="inlineStr">
@@ -12985,7 +12985,7 @@
       </c>
       <c r="F451" t="inlineStr">
         <is>
-          <t>MORRISON &amp; FOERSTER LLC</t>
+          <t>MORRISON &amp; FOERSTER</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -13265,7 +13265,7 @@
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t>VELEZ SECURITY SOLUTIONS LLC</t>
+          <t>VELEZ SECURITY SOLUTIONS</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -13464,7 +13464,7 @@
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t>WHITE &amp; CASE LLP</t>
+          <t>WHITE &amp; CASE</t>
         </is>
       </c>
       <c r="H468" t="inlineStr">
@@ -13550,7 +13550,7 @@
       </c>
       <c r="F471" t="inlineStr">
         <is>
-          <t>SUMS 15 HOLDINGS LLC</t>
+          <t>SUMS 15 HOLDINGS</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -13835,7 +13835,7 @@
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t>FACEBOOK INC</t>
+          <t>FACEBOOK</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -14233,7 +14233,7 @@
       </c>
       <c r="F495" t="inlineStr">
         <is>
-          <t>SIDLEY AUSTIN LLP</t>
+          <t>SIDLEY AUSTIN</t>
         </is>
       </c>
       <c r="H495" t="inlineStr">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="F496" t="inlineStr">
         <is>
-          <t>AIRBNB INC</t>
+          <t>AIRBNB</t>
         </is>
       </c>
       <c r="H496" t="inlineStr">
@@ -14459,7 +14459,7 @@
       </c>
       <c r="F503" t="inlineStr">
         <is>
-          <t>SEQUOIA CAPITAL OPERATIONS LLC</t>
+          <t>SEQUOIA CAPITAL OPERATIONS</t>
         </is>
       </c>
       <c r="H503" t="inlineStr">
@@ -14668,7 +14668,7 @@
       </c>
       <c r="F510" t="inlineStr">
         <is>
-          <t>LYFT INC</t>
+          <t>LYFT</t>
         </is>
       </c>
       <c r="H510" t="inlineStr">
@@ -14754,7 +14754,7 @@
       </c>
       <c r="F513" t="inlineStr">
         <is>
-          <t>AIRBNB INC</t>
+          <t>AIRBNB</t>
         </is>
       </c>
       <c r="H513" t="inlineStr">
@@ -14781,7 +14781,7 @@
       </c>
       <c r="F514" t="inlineStr">
         <is>
-          <t>MEOW WOLF INC</t>
+          <t>MEOW WOLF</t>
         </is>
       </c>
       <c r="H514" t="inlineStr">
@@ -15044,7 +15044,7 @@
       </c>
       <c r="F523" t="inlineStr">
         <is>
-          <t>LEVY GROUP INC</t>
+          <t>LEVY GROUP</t>
         </is>
       </c>
       <c r="H523" t="inlineStr">
@@ -15319,7 +15319,7 @@
       </c>
       <c r="F533" t="inlineStr">
         <is>
-          <t>COVINGTON &amp; BURLING LLP</t>
+          <t>COVINGTON &amp; BURLING</t>
         </is>
       </c>
       <c r="H533" t="inlineStr">
@@ -15936,7 +15936,7 @@
       </c>
       <c r="F554" t="inlineStr">
         <is>
-          <t>VISA INC</t>
+          <t>VISA</t>
         </is>
       </c>
       <c r="H554" t="inlineStr">
@@ -16221,7 +16221,7 @@
       </c>
       <c r="F564" t="inlineStr">
         <is>
-          <t>FUTURE PARTNERS LLC</t>
+          <t>FUTURE PARTNERS</t>
         </is>
       </c>
       <c r="H564" t="inlineStr">
@@ -16464,7 +16464,7 @@
       </c>
       <c r="F573" t="inlineStr">
         <is>
-          <t>FACEBOOK INC</t>
+          <t>FACEBOOK</t>
         </is>
       </c>
       <c r="H573" t="inlineStr">
@@ -16727,7 +16727,7 @@
       </c>
       <c r="F582" t="inlineStr">
         <is>
-          <t>JUGGERNAUT LLC</t>
+          <t>JUGGERNAUT</t>
         </is>
       </c>
       <c r="H582" t="inlineStr">
@@ -17142,7 +17142,7 @@
       </c>
       <c r="F597" t="inlineStr">
         <is>
-          <t>NATIONAL RESOURCES DEFENSE COUNCIL INC</t>
+          <t>NATIONAL RESOURCES DEFENSE COUNCIL</t>
         </is>
       </c>
       <c r="H597" t="inlineStr">
@@ -17169,7 +17169,7 @@
       </c>
       <c r="F598" t="inlineStr">
         <is>
-          <t>BANDERA ELECTRIC COOPERATIVE INC</t>
+          <t>BANDERA ELECTRIC COOPERATIVE</t>
         </is>
       </c>
       <c r="H598" t="inlineStr">
@@ -17572,7 +17572,7 @@
       </c>
       <c r="F612" t="inlineStr">
         <is>
-          <t>TRUEPIC INC</t>
+          <t>TRUEPIC</t>
         </is>
       </c>
       <c r="H612" t="inlineStr">

</xml_diff>